<commit_message>
Added code to adjust excel column widths
</commit_message>
<xml_diff>
--- a/Output/PyCitySchools_Output.xlsx
+++ b/Output/PyCitySchools_Output.xlsx
@@ -429,14 +429,29 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:L17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="8" max="8"/>
+    <col width="17" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="10" max="10"/>
+    <col width="29" customWidth="1" min="11" max="11"/>
+    <col width="18" customWidth="1" min="12" max="12"/>
+  </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
@@ -1290,14 +1305,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="17" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
@@ -1383,14 +1409,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:J15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="8" max="8"/>
+    <col width="17" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="10" max="10"/>
+  </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
@@ -1653,6 +1692,8 @@
         <v>90.54054054054053</v>
       </c>
     </row>
+    <row r="8"/>
+    <row r="9"/>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
@@ -1926,14 +1967,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="17" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
         <is>
@@ -2241,6 +2290,8 @@
         <v>83.6449864498645</v>
       </c>
     </row>
+    <row r="18"/>
+    <row r="19"/>
     <row r="20">
       <c r="B20" s="1" t="inlineStr">
         <is>
@@ -2559,14 +2610,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="29" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="17" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
@@ -2687,6 +2747,8 @@
         <v>53.5268548869691</v>
       </c>
     </row>
+    <row r="7"/>
+    <row r="8"/>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
@@ -2785,6 +2847,8 @@
         <v>58.28600304906789</v>
       </c>
     </row>
+    <row r="13"/>
+    <row r="14"/>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Added title outputs into excel sheets
</commit_message>
<xml_diff>
--- a/Output/PyCitySchools_Output.xlsx
+++ b/Output/PyCitySchools_Output.xlsx
@@ -451,7 +451,13 @@
     <col width="18" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Overall School Data</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
@@ -1323,7 +1329,13 @@
     <col width="17" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>District Summary</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
@@ -1429,7 +1441,13 @@
     <col width="18" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Highest-Performing Schools (by % Overall Passing)</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
@@ -1693,7 +1711,13 @@
       </c>
     </row>
     <row r="8"/>
-    <row r="9"/>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Lowest-Performing Schools (by % Overall Passing)</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
@@ -1982,7 +2006,13 @@
     <col width="17" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Math Scores by Grade</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
         <is>
@@ -2291,7 +2321,13 @@
       </c>
     </row>
     <row r="18"/>
-    <row r="19"/>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Reading Scores by Grade</t>
+        </is>
+      </c>
+    </row>
     <row r="20">
       <c r="B20" s="1" t="inlineStr">
         <is>
@@ -2626,7 +2662,13 @@
     <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Scores by School Spending</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
@@ -2748,7 +2790,13 @@
       </c>
     </row>
     <row r="7"/>
-    <row r="8"/>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Scores by School Size</t>
+        </is>
+      </c>
+    </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
@@ -2848,7 +2896,13 @@
       </c>
     </row>
     <row r="13"/>
-    <row r="14"/>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Scores by School Type</t>
+        </is>
+      </c>
+    </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>

</xml_diff>